<commit_message>
refactor: changed a lot of formulations
</commit_message>
<xml_diff>
--- a/chat/interview/questions.xlsx
+++ b/chat/interview/questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nordaxon-my.sharepoint.com/personal/melina_katkic_nordaxon_com/Documents/NORDAXON/AI ML PROJECTS/Emely/Intervjutips/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsabellaGagner\Documents\Programming-projects\emely\EmelyBackend\chat\interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1009" documentId="11_F25DC773A252ABDACC104857E15A47D45BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1CA9316A-7AF7-47B0-8C9E-FC5621ADB122}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2030CB7-4189-408E-841E-F123E55D6E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="8472" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45972" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,15 +72,6 @@
     <t>Kan du berätta om vad som motiverar dig när du arbetar?</t>
   </si>
   <si>
-    <t>Hur tycker du att en bra chef ska vara?</t>
-  </si>
-  <si>
-    <t>Finns det några speciella egenskaper du tycker att en bra chef ska ha?</t>
-  </si>
-  <si>
-    <t>Hur är du som arbetskamrat?</t>
-  </si>
-  <si>
     <t>Lagerarbetare</t>
   </si>
   <si>
@@ -90,12 +81,6 @@
     <t>Vilken inställning har du till att arbeta i grupp?</t>
   </si>
   <si>
-    <t>Varför ska vi anställa just dig?</t>
-  </si>
-  <si>
-    <t>Varför har du sökt det här arbetet?</t>
-  </si>
-  <si>
     <t>Hur reagerar du när du hamnar under tidspress?</t>
   </si>
   <si>
@@ -288,9 +273,6 @@
     <t>Är fastighetsteknik något du har erfarenhet av?</t>
   </si>
   <si>
-    <t>Har du någon tidigare erfarenhet inom vård?</t>
-  </si>
-  <si>
     <t>Är vård något du har arbetat med tidigare?</t>
   </si>
   <si>
@@ -408,30 +390,12 @@
     <t>Jag förstår. Låt oss nu tänka att du får den här tjänsten.</t>
   </si>
   <si>
-    <t>Tack, det låter bra. Angående din framtida chef.</t>
-  </si>
-  <si>
-    <t>Vad bra. Om du skulle beskriva dig själv.</t>
-  </si>
-  <si>
     <t>Nu tar vi nästa fråga.</t>
   </si>
   <si>
     <t>Det är viktigt att kunna jobba med andra.</t>
   </si>
   <si>
-    <t>Okej. Om vi tänker oss att det finns mycket att göra.</t>
-  </si>
-  <si>
-    <t>Bra svarat. Men nu skulle jag vilja veta.</t>
-  </si>
-  <si>
-    <t>Om vi nu funderar på vad som motiverar dig.</t>
-  </si>
-  <si>
-    <t>Tack! En annan fråga.</t>
-  </si>
-  <si>
     <t>Hur kommer det sig att du letar efter ett nytt jobb?</t>
   </si>
   <si>
@@ -444,24 +408,12 @@
     <t>Vad får dig att vara motiverad med dina arbetsuppgifter?</t>
   </si>
   <si>
-    <t>Är det något speciellt du skulle uppskatta av en chef?</t>
-  </si>
-  <si>
     <t>Tycker du om att ha egna arbetsuppgifter?</t>
   </si>
   <si>
     <t>Vad tycker du om grupparbete och samarbete med arbetskamrater?</t>
   </si>
   <si>
-    <t>Blir du lätt stressad?</t>
-  </si>
-  <si>
-    <t>Finns det något viktigt som du tror att du kan bidra med till vår verksamhet?</t>
-  </si>
-  <si>
-    <t>Vad kan du tillföra vår verksamhet?</t>
-  </si>
-  <si>
     <t>Vad gör du när du blir stressad?</t>
   </si>
   <si>
@@ -516,18 +468,12 @@
     <t>Har du jobbat med kassasystem tidigare, eller med något liknande?</t>
   </si>
   <si>
-    <t>Beskriv ett bra kundbemötande.</t>
-  </si>
-  <si>
     <t>Känner du till redovisningssystem, och hur de fungerar?</t>
   </si>
   <si>
     <t>Nu skulle jag vilja veta lite mer om dig.</t>
   </si>
   <si>
-    <t>Intressant. Nu skulle jag vilja veta lite mer om dig.</t>
-  </si>
-  <si>
     <t>Jag förstår. Nu vill jag veta lite om ditt arbetssätt.</t>
   </si>
   <si>
@@ -537,9 +483,6 @@
     <t>Min nästa fråga, i butik är bemötandet viktigt.</t>
   </si>
   <si>
-    <t>Bra svarat. Som ekonomiassistent är redovisning viktigt.</t>
-  </si>
-  <si>
     <t>Har du arbetat med olika typer av fordon?</t>
   </si>
   <si>
@@ -645,12 +588,6 @@
     <t>Har du någon erfarenhet av städning?</t>
   </si>
   <si>
-    <t>Jag förstår. Som lokalvårdare är städning viktigt.</t>
-  </si>
-  <si>
-    <t>Bra svarat. Nu vill jag veta lite om dina kvalifikationer som lärare.</t>
-  </si>
-  <si>
     <t>Har du arbetat som lärare tidigare?</t>
   </si>
   <si>
@@ -690,9 +627,6 @@
     <t>Vilken inriktning har du som sjuksköterska?</t>
   </si>
   <si>
-    <t>Hur skulle du beskriva ett bra bemötande?</t>
-  </si>
-  <si>
     <t>Har du någon erfarenhet av olika typer av snickeri?</t>
   </si>
   <si>
@@ -723,12 +657,6 @@
     <t>Okej, nu vill jag prata lite om vad du tycker är viktigt som receptionist.</t>
   </si>
   <si>
-    <t xml:space="preserve">Jaha, okej. Som receptionist finns flera arbetsuppgifter. </t>
-  </si>
-  <si>
-    <t>Vad bra. Som servitör arbetar men mycket med kassa.</t>
-  </si>
-  <si>
     <t>Bra svarat!</t>
   </si>
   <si>
@@ -741,9 +669,6 @@
     <t>Tack för de svaren. Tandsköterska är ju ett vårdyrke.</t>
   </si>
   <si>
-    <t>Okej. Men när det gäller specifikt jobbet som tandsköterska.</t>
-  </si>
-  <si>
     <t>Intressant! Nu vill jag veta lite mer om dina erfarenheter.</t>
   </si>
   <si>
@@ -753,12 +678,6 @@
     <t>Tack! Många vårdassistenter jobbar mycket med äldre.</t>
   </si>
   <si>
-    <t>Vad tror du att andra tycker om dig som kollega?</t>
-  </si>
-  <si>
-    <t>Hur tror du att du skulle vara som kollega?</t>
-  </si>
-  <si>
     <t>Vilka situationer får dig att bli stressad?</t>
   </si>
   <si>
@@ -766,6 +685,87 @@
   </si>
   <si>
     <t>Vad brukar du göra när du är ledig?</t>
+  </si>
+  <si>
+    <t>hur tycker du att en bra chef ska vara?</t>
+  </si>
+  <si>
+    <t>finns det några speciella egenskaper du tycker att en bra chef ska ha?</t>
+  </si>
+  <si>
+    <t>är det något speciellt du skulle uppskatta hos en chef?</t>
+  </si>
+  <si>
+    <t>Tack, det låter bra. När det gäller chefer,</t>
+  </si>
+  <si>
+    <t>som arbetskamrat, vad skulle du säga då?</t>
+  </si>
+  <si>
+    <t>hur tror du att du skulle vara som kollega?</t>
+  </si>
+  <si>
+    <t>Vad bra. Om du skulle beskriva dig själv,</t>
+  </si>
+  <si>
+    <t>vad skulle du tro att andra tycker om dig som kollega?</t>
+  </si>
+  <si>
+    <t>Okej. Nu ska vi prata lite om stress och hur det påverkar dig.</t>
+  </si>
+  <si>
+    <t>varför vi ska anställa just dig?</t>
+  </si>
+  <si>
+    <t>vad du kan tillföra vår verksamhet?</t>
+  </si>
+  <si>
+    <t>om det finns något speciellt som du tror att du kan bidra med till vår verksamhet?</t>
+  </si>
+  <si>
+    <t>Okej, jag förstår. Men nu skulle jag vilja veta</t>
+  </si>
+  <si>
+    <t>Om vi nu funderar på vad som intresserar dig.</t>
+  </si>
+  <si>
+    <t>Varför har du sökt just det här arbetet?</t>
+  </si>
+  <si>
+    <t>Tack! En annan fråga gällande stress.</t>
+  </si>
+  <si>
+    <t>När brukar du känna dig stressad?</t>
+  </si>
+  <si>
+    <t>Intressant. Jag skulle vilja veta lite mer om dig.</t>
+  </si>
+  <si>
+    <t>Kan du beskriva vad du tycker är ett bra kundbemötande?</t>
+  </si>
+  <si>
+    <t>Tack för det. Som ekonomiassistent är redovisning viktigt.</t>
+  </si>
+  <si>
+    <t>Jag förstår. Som lokalvårdare är ordning och reda viktigt.</t>
+  </si>
+  <si>
+    <t>Tack för det svaret. Nu vill jag veta lite om dina kvalifikationer som lärare.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ja, okej. Som receptionist finns flera arbetsuppgifter. </t>
+  </si>
+  <si>
+    <t>Vad bra. Som servitör arbetar man mycket med kassan.</t>
+  </si>
+  <si>
+    <t>Hur skulle du beskriva ett bra patientbemötande?</t>
+  </si>
+  <si>
+    <t>Har du någon annan erfarenhet inom vården?</t>
+  </si>
+  <si>
+    <t>Okej. När det gäller jobbet som tandsköterska.</t>
   </si>
 </sst>
 </file>
@@ -1484,8 +1484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="K54" sqref="K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1506,37 +1506,37 @@
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>115</v>
-      </c>
       <c r="H1" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1562,7 +1562,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>1</v>
@@ -1597,7 +1597,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>4</v>
@@ -1606,7 +1606,7 @@
         <v>5</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1632,16 +1632,16 @@
         <v>0</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>118</v>
+        <v>214</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>6</v>
+        <v>211</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>7</v>
+        <v>212</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>130</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1667,16 +1667,16 @@
         <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>119</v>
+        <v>217</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>8</v>
+        <v>215</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1702,16 +1702,16 @@
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1737,16 +1737,16 @@
         <v>1</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1772,16 +1772,16 @@
         <v>0</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>122</v>
+        <v>219</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>235</v>
+        <v>208</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>133</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1807,16 +1807,16 @@
         <v>1</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>123</v>
+        <v>223</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>12</v>
+        <v>220</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>135</v>
+        <v>221</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>134</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1842,16 +1842,16 @@
         <v>0</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>124</v>
+        <v>224</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>13</v>
+        <v>225</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>236</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1877,16 +1877,16 @@
         <v>0</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>125</v>
+        <v>226</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1912,16 +1912,16 @@
         <v>1</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1947,16 +1947,16 @@
         <v>0</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1982,16 +1982,16 @@
         <v>0</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2017,16 +2017,16 @@
         <v>1</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2052,16 +2052,16 @@
         <v>1</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>237</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2087,21 +2087,21 @@
         <v>1</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>157</v>
+        <v>228</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -2122,21 +2122,21 @@
         <v>1</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
@@ -2157,21 +2157,21 @@
         <v>0</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
@@ -2192,21 +2192,21 @@
         <v>0</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B21" s="1">
         <v>0</v>
@@ -2227,21 +2227,21 @@
         <v>1</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
@@ -2262,21 +2262,21 @@
         <v>1</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B23" s="1">
         <v>0</v>
@@ -2297,21 +2297,21 @@
         <v>0</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B24" s="1">
         <v>0</v>
@@ -2332,21 +2332,21 @@
         <v>1</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
@@ -2367,21 +2367,21 @@
         <v>0</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>154</v>
+        <v>229</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
@@ -2402,21 +2402,21 @@
         <v>1</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>161</v>
+        <v>230</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
@@ -2437,21 +2437,21 @@
         <v>1</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B28" s="1">
         <v>1</v>
@@ -2472,21 +2472,21 @@
         <v>0</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B29" s="1">
         <v>1</v>
@@ -2507,21 +2507,21 @@
         <v>0</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
@@ -2542,21 +2542,21 @@
         <v>1</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
@@ -2577,21 +2577,21 @@
         <v>0</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B32" s="1">
         <v>0</v>
@@ -2612,21 +2612,21 @@
         <v>1</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B33" s="1">
         <v>0</v>
@@ -2647,21 +2647,21 @@
         <v>1</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B34" s="1">
         <v>0</v>
@@ -2682,21 +2682,21 @@
         <v>1</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B35" s="1">
         <v>0</v>
@@ -2717,21 +2717,21 @@
         <v>1</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B36" s="1">
         <v>0</v>
@@ -2752,21 +2752,21 @@
         <v>0</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="29.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B37" s="1">
         <v>0</v>
@@ -2787,21 +2787,21 @@
         <v>0</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B38" s="1">
         <v>0</v>
@@ -2822,21 +2822,21 @@
         <v>0</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B39" s="1">
         <v>0</v>
@@ -2857,21 +2857,21 @@
         <v>1</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B40" s="1">
         <v>0</v>
@@ -2892,21 +2892,21 @@
         <v>1</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B41" s="1">
         <v>0</v>
@@ -2927,21 +2927,21 @@
         <v>1</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>222</v>
+        <v>200</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B42" s="1">
         <v>1</v>
@@ -2962,21 +2962,21 @@
         <v>0</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B43" s="1">
         <v>0</v>
@@ -2997,21 +2997,21 @@
         <v>0</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B44" s="1">
         <v>0</v>
@@ -3032,21 +3032,21 @@
         <v>0</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B45" s="1">
         <v>0</v>
@@ -3067,21 +3067,21 @@
         <v>0</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B46" s="1">
         <v>0</v>
@@ -3102,21 +3102,21 @@
         <v>0</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>212</v>
+        <v>235</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B47" s="1">
         <v>0</v>
@@ -3137,21 +3137,21 @@
         <v>0</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>227</v>
+        <v>203</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>213</v>
+        <v>191</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B48" s="1">
         <v>0</v>
@@ -3172,21 +3172,21 @@
         <v>0</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>214</v>
+        <v>192</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B49" s="1">
         <v>0</v>
@@ -3207,21 +3207,21 @@
         <v>0</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>78</v>
+        <v>236</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B50" s="1">
         <v>1</v>
@@ -3242,21 +3242,21 @@
         <v>0</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B51" s="1">
         <v>0</v>
@@ -3277,21 +3277,21 @@
         <v>0</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>216</v>
+        <v>194</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>217</v>
+        <v>195</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B52" s="1">
         <v>0</v>
@@ -3312,21 +3312,21 @@
         <v>0</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>231</v>
+        <v>206</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>218</v>
+        <v>196</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B53" s="1">
         <v>0</v>
@@ -3347,21 +3347,21 @@
         <v>0</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>219</v>
+        <v>197</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B54" s="1">
         <v>0</v>
@@ -3382,16 +3382,16 @@
         <v>0</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>220</v>
+        <v>198</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>221</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: changed interview questions back to full sentences
</commit_message>
<xml_diff>
--- a/chat/interview/questions.xlsx
+++ b/chat/interview/questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsabellaGagner\Documents\Programming-projects\emely\EmelyBackend\chat\interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2030CB7-4189-408E-841E-F123E55D6E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9D86E1-941C-4E6B-A901-AC4CBC124345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -687,45 +687,9 @@
     <t>Vad brukar du göra när du är ledig?</t>
   </si>
   <si>
-    <t>hur tycker du att en bra chef ska vara?</t>
-  </si>
-  <si>
-    <t>finns det några speciella egenskaper du tycker att en bra chef ska ha?</t>
-  </si>
-  <si>
-    <t>är det något speciellt du skulle uppskatta hos en chef?</t>
-  </si>
-  <si>
-    <t>Tack, det låter bra. När det gäller chefer,</t>
-  </si>
-  <si>
-    <t>som arbetskamrat, vad skulle du säga då?</t>
-  </si>
-  <si>
-    <t>hur tror du att du skulle vara som kollega?</t>
-  </si>
-  <si>
-    <t>Vad bra. Om du skulle beskriva dig själv,</t>
-  </si>
-  <si>
-    <t>vad skulle du tro att andra tycker om dig som kollega?</t>
-  </si>
-  <si>
     <t>Okej. Nu ska vi prata lite om stress och hur det påverkar dig.</t>
   </si>
   <si>
-    <t>varför vi ska anställa just dig?</t>
-  </si>
-  <si>
-    <t>vad du kan tillföra vår verksamhet?</t>
-  </si>
-  <si>
-    <t>om det finns något speciellt som du tror att du kan bidra med till vår verksamhet?</t>
-  </si>
-  <si>
-    <t>Okej, jag förstår. Men nu skulle jag vilja veta</t>
-  </si>
-  <si>
     <t>Om vi nu funderar på vad som intresserar dig.</t>
   </si>
   <si>
@@ -766,6 +730,42 @@
   </si>
   <si>
     <t>Okej. När det gäller jobbet som tandsköterska.</t>
+  </si>
+  <si>
+    <t>Tack, det låter bra. När det gäller chefer..</t>
+  </si>
+  <si>
+    <t>Hur tycker du att en bra chef ska vara?</t>
+  </si>
+  <si>
+    <t>Finns det några speciella egenskaper du tycker att en bra chef ska ha?</t>
+  </si>
+  <si>
+    <t>Är det något speciellt du skulle uppskatta hos en chef?</t>
+  </si>
+  <si>
+    <t>Om du skulle beskriva dig själv som arbetskamrat, vad skulle du säga då?</t>
+  </si>
+  <si>
+    <t>Om du skulle beskriva dig själv, hur tror du att du skulle vara som kollega?</t>
+  </si>
+  <si>
+    <t>Vad tänker du att du kan tillföra vår verksamhet?</t>
+  </si>
+  <si>
+    <t>Finns det något speciellt som du tror att du kan bidra med till vår verksamhet?</t>
+  </si>
+  <si>
+    <t>Jag skulle vilja veta varför du tycker att vi ska anställa just dig?</t>
+  </si>
+  <si>
+    <t>Okej, jag förstår. Vi går vidare.</t>
+  </si>
+  <si>
+    <t>Vad bra. Nu kommer jag ställa en fråga om dig som arbetskamrat.</t>
+  </si>
+  <si>
+    <t>Vad skulle du tro att andra tycker om dig som kollega?</t>
   </si>
 </sst>
 </file>
@@ -1484,27 +1484,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="K54" sqref="K54"/>
+    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.3125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.68359375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83984375" style="1"/>
+    <col min="1" max="1" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="1"/>
     <col min="5" max="5" width="10" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.3125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="42.41796875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="41.5234375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="37.15625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="37.05078125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.83984375" style="1"/>
+    <col min="6" max="6" width="11.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="42.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="41.5546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="37.109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="37" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>99</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1632,19 +1632,19 @@
         <v>0</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>212</v>
+        <v>228</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1667,19 +1667,19 @@
         <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>217</v>
+        <v>236</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>208</v>
@@ -1781,10 +1781,10 @@
         <v>87</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1807,19 +1807,19 @@
         <v>1</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>220</v>
+        <v>234</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1842,10 +1842,10 @@
         <v>0</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>41</v>
@@ -1854,7 +1854,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>9</v>
@@ -1889,7 +1889,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>1</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>151</v>
@@ -2099,7 +2099,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>16</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>17</v>
       </c>
@@ -2376,10 +2376,10 @@
         <v>61</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>18</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>1</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>76</v>
@@ -2414,7 +2414,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>18</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>19</v>
       </c>
@@ -2484,7 +2484,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>19</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>6</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>20</v>
       </c>
@@ -2624,7 +2624,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>20</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>21</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>21</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>1</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>92</v>
@@ -2729,7 +2729,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>22</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>0</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>35</v>
@@ -2764,7 +2764,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="29.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:11" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>22</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>22</v>
       </c>
@@ -2834,7 +2834,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>23</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>23</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>24</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>24</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>0</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>80</v>
@@ -2974,7 +2974,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>25</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>25</v>
       </c>
@@ -3032,7 +3032,7 @@
         <v>0</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>78</v>
@@ -3044,7 +3044,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>26</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>26</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>202</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>84</v>
@@ -3114,7 +3114,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>27</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>27</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>28</v>
       </c>
@@ -3210,7 +3210,7 @@
         <v>204</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>73</v>
@@ -3219,7 +3219,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>28</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>0</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>74</v>
@@ -3254,7 +3254,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>29</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>29</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>30</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>30</v>
       </c>

</xml_diff>